<commit_message>
Modificación a la fecha y hora de actualización
</commit_message>
<xml_diff>
--- a/Resources/data/Versión_7.0/Version_7.0.xlsx
+++ b/Resources/data/Versión_7.0/Version_7.0.xlsx
@@ -6727,7 +6727,7 @@
   <dimension ref="A1:N48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
@@ -7077,7 +7077,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="9" s="24" customFormat="1" ht="25" customHeight="1" spans="1:14">
+    <row r="9" s="24" customFormat="1" ht="25" hidden="1" customHeight="1" spans="1:14">
       <c r="A9" s="29" t="s">
         <v>387</v>
       </c>
@@ -7121,7 +7121,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="10" s="25" customFormat="1" ht="25" customHeight="1" spans="1:14">
+    <row r="10" s="25" customFormat="1" ht="25" hidden="1" customHeight="1" spans="1:14">
       <c r="A10" s="33" t="s">
         <v>387</v>
       </c>
@@ -7165,7 +7165,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="11" s="24" customFormat="1" ht="25" customHeight="1" spans="1:14">
+    <row r="11" s="24" customFormat="1" ht="25" hidden="1" customHeight="1" spans="1:14">
       <c r="A11" s="29" t="s">
         <v>387</v>
       </c>
@@ -7209,7 +7209,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="12" s="24" customFormat="1" ht="25" customHeight="1" spans="1:14">
+    <row r="12" s="24" customFormat="1" ht="25" hidden="1" customHeight="1" spans="1:14">
       <c r="A12" s="29" t="s">
         <v>387</v>
       </c>
@@ -7605,7 +7605,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="21" s="25" customFormat="1" ht="25" customHeight="1" spans="1:14">
+    <row r="21" s="25" customFormat="1" ht="25" hidden="1" customHeight="1" spans="1:14">
       <c r="A21" s="33" t="s">
         <v>387</v>
       </c>
@@ -7649,7 +7649,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="22" s="25" customFormat="1" ht="25" customHeight="1" spans="1:14">
+    <row r="22" s="25" customFormat="1" ht="25" hidden="1" customHeight="1" spans="1:14">
       <c r="A22" s="33" t="s">
         <v>387</v>
       </c>
@@ -7957,7 +7957,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="29" s="24" customFormat="1" ht="25" hidden="1" customHeight="1" spans="1:14">
+    <row r="29" s="24" customFormat="1" ht="25" customHeight="1" spans="1:14">
       <c r="A29" s="29" t="s">
         <v>449</v>
       </c>
@@ -8001,7 +8001,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="30" s="24" customFormat="1" ht="25" hidden="1" customHeight="1" spans="1:14">
+    <row r="30" s="24" customFormat="1" ht="25" customHeight="1" spans="1:14">
       <c r="A30" s="29" t="s">
         <v>449</v>
       </c>
@@ -8045,7 +8045,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="31" s="26" customFormat="1" ht="25" hidden="1" customHeight="1" spans="1:14">
+    <row r="31" s="26" customFormat="1" ht="25" customHeight="1" spans="1:14">
       <c r="A31" s="29" t="s">
         <v>449</v>
       </c>
@@ -8089,7 +8089,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="32" s="26" customFormat="1" ht="25" hidden="1" customHeight="1" spans="1:14">
+    <row r="32" s="26" customFormat="1" ht="25" customHeight="1" spans="1:14">
       <c r="A32" s="29" t="s">
         <v>449</v>
       </c>
@@ -8133,7 +8133,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="33" s="26" customFormat="1" ht="25" hidden="1" customHeight="1" spans="1:14">
+    <row r="33" s="26" customFormat="1" ht="25" customHeight="1" spans="1:14">
       <c r="A33" s="29" t="s">
         <v>449</v>
       </c>
@@ -8177,7 +8177,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="34" s="24" customFormat="1" ht="25" hidden="1" customHeight="1" spans="1:14">
+    <row r="34" s="24" customFormat="1" ht="25" customHeight="1" spans="1:14">
       <c r="A34" s="29" t="s">
         <v>449</v>
       </c>
@@ -8273,7 +8273,7 @@
   <autoFilter ref="A2:N34">
     <filterColumn colId="0">
       <customFilters>
-        <customFilter operator="equal" val="Gerardo"/>
+        <customFilter operator="equal" val="Blanca"/>
       </customFilters>
     </filterColumn>
     <extLst/>

</xml_diff>